<commit_message>
Added varying text scroll speeds
Text in dialogue can no scroll at different speeds.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/episode1_cutscene1.xlsx
+++ b/Typocrypha/Assets/excel/episode1_cutscene1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="30">
   <si>
     <t>START_SCENE</t>
   </si>
@@ -47,15 +47,6 @@
     <t>Player</t>
   </si>
   <si>
-    <t>. . .</t>
-  </si>
-  <si>
-    <t>Uh . . . Is this thing on?</t>
-  </si>
-  <si>
-    <t>( . . . Crap. I just got this thing too)</t>
-  </si>
-  <si>
     <t>???</t>
   </si>
   <si>
@@ -71,46 +62,58 @@
     <t>Welcome back (Uncle name here)! You last activated this &lt;color=blue&gt;TYPOCRYPHA&lt;/color&gt; unit 1 year, 1 month, and 13 days ago. You have &lt;color=yellow&gt;1023&lt;/color&gt; new updates and &lt;color=yellow&gt;33,333&lt;/color&gt; new emails.</t>
   </si>
   <si>
-    <t>[block=t]NonononoNONON-[fade=out,0,0,0,0][pause=3][next]</t>
-  </si>
-  <si>
-    <t>[fade=in,2,0,0,0]REINITIALIZING . . . [pause=3][next]</t>
-  </si>
-  <si>
     <t>. . . Maybe?</t>
   </si>
   <si>
     <t>Technology sucks.</t>
   </si>
   <si>
-    <t>&lt;size=48&gt;[play-sfx=take_damage][screen-shake=0.2,0.3]THWACK . . . [play-sfx=take_damage][screen-shake=0.2,0.3]WHAM . . .&lt;/size&gt;</t>
-  </si>
-  <si>
     <t>O-Oh. No, Im not [Uncles name]. I-uh . . . Dammit! How do I reset-</t>
   </si>
   <si>
-    <t>[block=t]click . . .[pause=1] click[pause=0.5] click[pause=0.5][block=f]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[block=f]OK . . . I think I fixed it. </t>
-  </si>
-  <si>
-    <t>. . . Uh, hel-</t>
-  </si>
-  <si>
     <t>Thank you for purchasing this &lt;color=blue&gt;TYPOCRYPHA&lt;/color&gt; unit. I will be your AI operating assistant.</t>
   </si>
   <si>
     <t>You can call me Clarke!</t>
   </si>
   <si>
-    <t>Uh, hi Cla-</t>
-  </si>
-  <si>
     <t>Clarke</t>
   </si>
   <si>
     <t>What's your name?</t>
+  </si>
+  <si>
+    <t>[set-scroll-delay=0.05]. . .</t>
+  </si>
+  <si>
+    <t>(Maybe if I just . . . )</t>
+  </si>
+  <si>
+    <t>[block=t]NonononoNONON[fade=out,0,0,0,0][pause=3][next]</t>
+  </si>
+  <si>
+    <t>[set-scroll-delay=0.3]. . . [set-scroll-delay=0.05] Did-[pause=0.5]Did it wo[next]</t>
+  </si>
+  <si>
+    <t>[block=t][set-scroll-delay=0]&lt;size=48&gt;[play-sfx=take_damage][screen-shake=0.2,0.3]THWACK!![pause=1]     [play-sfx=take_damage][screen-shake=0.2,0.3]WHAM!!&lt;/size&gt;[set-scroll-delay=0.05][block=f]</t>
+  </si>
+  <si>
+    <t>Uh . . .[pause=1] Is this thing on?</t>
+  </si>
+  <si>
+    <t>( . . . Crap. I just got this thing too.)</t>
+  </si>
+  <si>
+    <t>[fade=in,1.5,0,0,0]REINITIALIZING . . . [pause=3][next]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[block=f]OK . . . [pause=1]I think I fixed it. </t>
+  </si>
+  <si>
+    <t>[set-scroll-delay=0.3]. . . [set-scroll-delay=0.05] Uh,[pause=0.5] hel[next]</t>
+  </si>
+  <si>
+    <t>[block=t][set-scroll-delay=0]click[set-scroll-delay=0.3] . . .[pause=1][set-scroll-delay=0] click.[pause=0.5] click.[pause=0.5][set-scroll-delay=0.05][block=f]</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +507,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -518,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -535,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
@@ -552,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -565,8 +568,11 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -579,11 +585,8 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -597,13 +600,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>3</v>
@@ -614,10 +617,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>5</v>
@@ -631,13 +634,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>3</v>
@@ -651,7 +654,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>3</v>
@@ -662,19 +668,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -682,10 +688,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>3</v>
@@ -696,10 +699,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
@@ -708,7 +711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -716,7 +719,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -733,7 +736,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -747,10 +750,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>5</v>
@@ -764,13 +767,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>3</v>
@@ -781,10 +784,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>5</v>
@@ -798,13 +801,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>3</v>
@@ -815,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>5</v>
@@ -829,6 +832,23 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Spruced up current episode 1 demo
Small changes to episode1_cutscene1 dialogue
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/episode1_cutscene1.xlsx
+++ b/Typocrypha/Assets/excel/episode1_cutscene1.xlsx
@@ -59,18 +59,12 @@
     <t>&lt;size=48&gt;&lt;color=red&gt;ERROR UNIDENTIFIED USER. FORCE SHUTTING DOWN . . .&lt;/color&gt;&lt;/size&gt;</t>
   </si>
   <si>
-    <t>Welcome back (Uncle name here)! You last activated this &lt;color=blue&gt;TYPOCRYPHA&lt;/color&gt; unit 1 year, 1 month, and 13 days ago. You have &lt;color=yellow&gt;1023&lt;/color&gt; new updates and &lt;color=yellow&gt;33,333&lt;/color&gt; new emails.</t>
-  </si>
-  <si>
     <t>. . . Maybe?</t>
   </si>
   <si>
     <t>Technology sucks.</t>
   </si>
   <si>
-    <t>O-Oh. No, Im not [Uncles name]. I-uh . . . Dammit! How do I reset-</t>
-  </si>
-  <si>
     <t>Thank you for purchasing this &lt;color=blue&gt;TYPOCRYPHA&lt;/color&gt; unit. I will be your AI operating assistant.</t>
   </si>
   <si>
@@ -114,6 +108,12 @@
   </si>
   <si>
     <t>[block=t][set-scroll-delay=0]click[set-scroll-delay=0.3] . . .[pause=1][set-scroll-delay=0] click.[pause=0.5] click.[pause=0.5][set-scroll-delay=0.05][block=f]</t>
+  </si>
+  <si>
+    <t>Welcome back Uncle Nintendo! You last activated this &lt;color=blue&gt;TYPOCRYPHA&lt;/color&gt; unit 1 year, 1 month, and 13 days ago. You have &lt;color=yellow&gt;1023&lt;/color&gt; new updates and &lt;color=yellow&gt;33,333&lt;/color&gt; new emails.</t>
+  </si>
+  <si>
+    <t>O-Oh. No, Im not him. I-uh . . . Dammit! How do I reset-</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,7 +507,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -538,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
@@ -555,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -572,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -586,7 +586,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
@@ -637,7 +637,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -654,7 +654,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
@@ -688,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>3</v>
@@ -702,7 +702,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
@@ -719,7 +719,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -736,7 +736,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -753,7 +753,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>5</v>
@@ -770,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>5</v>
@@ -804,7 +804,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -818,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>5</v>
@@ -835,10 +835,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>

</xml_diff>